<commit_message>
add clusters and new rules
</commit_message>
<xml_diff>
--- a/normalizing_rules.xlsx
+++ b/normalizing_rules.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t>from_normalize</t>
   </si>
@@ -87,6 +87,27 @@
   </si>
   <si>
     <t>(ch)+</t>
+  </si>
+  <si>
+    <t>p(i|e+)</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>di</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>bi</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>bichwala</t>
   </si>
 </sst>
 </file>
@@ -183,10 +204,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B13" activeCellId="0" pane="topLeft" sqref="B13"/>
+      <selection activeCell="A17" activeCellId="0" pane="topLeft" sqref="A17:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -304,6 +325,36 @@
         <v>13</v>
       </c>
     </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
+      <c r="A14" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="15">
+      <c r="A15" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="16">
+      <c r="A16" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="17"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="18"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="19"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>